<commit_message>
Arreglo en .py,graficos y docs
</commit_message>
<xml_diff>
--- a/Catalogo componentes y precios.xlsx
+++ b/Catalogo componentes y precios.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chus1\Downloads\Proyecto Máquinas Eléctricas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Vasquez\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E74B31B5-3CEF-4E5A-A17D-EC53B1209A67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E32C4FED-8DCE-4822-9F4D-5ACEA76EDF4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="1725" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Componentes" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,12 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="147">
   <si>
     <t>Protección</t>
   </si>
@@ -474,6 +471,9 @@
   </si>
   <si>
     <t>Transformador monofásico 19.9 kV / 277 V / 333 kVA</t>
+  </si>
+  <si>
+    <t>Darle potencia al recloser</t>
   </si>
 </sst>
 </file>
@@ -495,7 +495,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -505,6 +505,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -521,7 +533,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -542,6 +554,51 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -824,21 +881,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E139"/>
+  <dimension ref="A1:D139"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" zoomScale="138" workbookViewId="0">
+      <selection activeCell="C77" sqref="C77"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="88.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" customWidth="1"/>
+    <col min="1" max="1" width="22.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="88.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.6640625" customWidth="1"/>
+    <col min="5" max="5" width="12.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -849,18 +907,18 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="17" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="7">
         <v>1258</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -871,18 +929,21 @@
         <v>1332</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="16" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="7">
         <v>1482.65</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
@@ -893,7 +954,7 @@
         <v>1260</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
@@ -904,220 +965,225 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="19">
         <v>1164.5</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="21" t="s">
         <v>2</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="19">
         <v>1750</v>
       </c>
-      <c r="E8">
-        <f>2000*(5/600)</f>
-        <v>16.666666666666668</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="21" t="s">
         <v>2</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="19">
         <v>1854</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="19">
         <v>2039</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="D10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="21" t="s">
         <v>0</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="19">
         <v>86.4</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="21" t="s">
         <v>0</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="19">
         <v>69.8</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="21" t="s">
         <v>0</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="19">
         <v>88.492500000000007</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="21" t="s">
         <v>0</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="19">
         <v>106.75</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C15" s="19">
         <v>113.64</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="7">
+      <c r="C16" s="19">
         <v>113.64</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C17" s="19">
         <v>1.26</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="7">
+      <c r="C18" s="19">
         <v>1.6800000000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="7">
+      <c r="C19" s="19">
         <v>38.813333333333333</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="7">
+      <c r="C20" s="19">
         <v>51.5</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="7">
+      <c r="C21" s="19">
         <v>59.317499999999995</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
+      <c r="D21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="21" t="s">
         <v>1</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C22" s="7">
+      <c r="C22" s="19">
         <v>614.54999999999995</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="21" t="s">
         <v>1</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="7">
+      <c r="C23" s="19">
         <v>650.70000000000005</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="C24" s="7">
+      <c r="C24" s="19">
         <v>626.63</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="7">
+      <c r="C25" s="19">
         <v>191.25</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>1</v>
       </c>
@@ -1128,18 +1194,18 @@
         <v>202.5</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C27" s="7">
+      <c r="C27" s="10">
         <v>206.98</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>1</v>
       </c>
@@ -1150,7 +1216,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>1</v>
       </c>
@@ -1161,7 +1227,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>1</v>
       </c>
@@ -1172,7 +1238,7 @@
         <v>181.20999999999998</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>1</v>
       </c>
@@ -1183,7 +1249,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>1</v>
       </c>
@@ -1194,18 +1260,21 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B33" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="C33" s="7">
+      <c r="C33" s="19">
         <v>8000</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>3</v>
       </c>
@@ -1216,7 +1285,7 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>3</v>
       </c>
@@ -1227,7 +1296,7 @@
         <v>6735</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>3</v>
       </c>
@@ -1238,7 +1307,7 @@
         <v>6748</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>3</v>
       </c>
@@ -1249,7 +1318,7 @@
         <v>8200</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>3</v>
       </c>
@@ -1260,7 +1329,7 @@
         <v>11500</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>3</v>
       </c>
@@ -1271,7 +1340,7 @@
         <v>7071</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>3</v>
       </c>
@@ -1282,7 +1351,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>3</v>
       </c>
@@ -1293,7 +1362,7 @@
         <v>4800</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
         <v>3</v>
       </c>
@@ -1304,7 +1373,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
         <v>3</v>
       </c>
@@ -1315,7 +1384,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
         <v>3</v>
       </c>
@@ -1326,7 +1395,7 @@
         <v>6200</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
         <v>3</v>
       </c>
@@ -1337,7 +1406,7 @@
         <v>6500</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
         <v>3</v>
       </c>
@@ -1348,7 +1417,7 @@
         <v>6420.5</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
         <v>3</v>
       </c>
@@ -1359,7 +1428,7 @@
         <v>6200</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
         <v>3</v>
       </c>
@@ -1370,7 +1439,7 @@
         <v>6900</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
         <v>3</v>
       </c>
@@ -1381,7 +1450,7 @@
         <v>6778.67</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
         <v>3</v>
       </c>
@@ -1392,7 +1461,7 @@
         <v>6735</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
         <v>3</v>
       </c>
@@ -1403,7 +1472,7 @@
         <v>5409</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
         <v>3</v>
       </c>
@@ -1414,7 +1483,7 @@
         <v>14100</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
         <v>3</v>
       </c>
@@ -1425,7 +1494,7 @@
         <v>15400</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
         <v>3</v>
       </c>
@@ -1436,7 +1505,7 @@
         <v>17800</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
         <v>3</v>
       </c>
@@ -1447,7 +1516,7 @@
         <v>32028</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
         <v>3</v>
       </c>
@@ -1458,7 +1527,7 @@
         <v>32028</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
         <v>3</v>
       </c>
@@ -1469,7 +1538,7 @@
         <v>32028</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
         <v>3</v>
       </c>
@@ -1480,7 +1549,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
         <v>3</v>
       </c>
@@ -1491,7 +1560,7 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
         <v>3</v>
       </c>
@@ -1502,7 +1571,7 @@
         <v>15400</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
         <v>3</v>
       </c>
@@ -1513,7 +1582,7 @@
         <v>16598</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" s="3" t="s">
         <v>3</v>
       </c>
@@ -1524,7 +1593,7 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
         <v>3</v>
       </c>
@@ -1535,7 +1604,7 @@
         <v>15279</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" s="3" t="s">
         <v>3</v>
       </c>
@@ -1546,7 +1615,7 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
         <v>3</v>
       </c>
@@ -1557,7 +1626,7 @@
         <v>13500</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="s">
         <v>3</v>
       </c>
@@ -1568,7 +1637,7 @@
         <v>14800.5</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="s">
         <v>3</v>
       </c>
@@ -1579,40 +1648,40 @@
         <v>43387</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B68" s="1" t="s">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B68" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="C68" s="7">
+      <c r="C68" s="10">
         <v>43387</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B69" s="1" t="s">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A69" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B69" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="C69" s="7">
+      <c r="C69" s="19">
         <v>50815</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B70" s="1" t="s">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A70" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B70" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="C70" s="7">
+      <c r="C70" s="13">
         <v>50815</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" s="3" t="s">
         <v>3</v>
       </c>
@@ -1623,7 +1692,7 @@
         <v>16000</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" s="3" t="s">
         <v>3</v>
       </c>
@@ -1634,7 +1703,7 @@
         <v>18150</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" s="3" t="s">
         <v>3</v>
       </c>
@@ -1645,7 +1714,7 @@
         <v>16000</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" s="3" t="s">
         <v>3</v>
       </c>
@@ -1656,7 +1725,7 @@
         <v>18000</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" s="3" t="s">
         <v>3</v>
       </c>
@@ -1667,7 +1736,7 @@
         <v>18866.669999999998</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" s="3" t="s">
         <v>3</v>
       </c>
@@ -1678,7 +1747,7 @@
         <v>8500</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" s="3" t="s">
         <v>3</v>
       </c>
@@ -1689,7 +1758,7 @@
         <v>8500</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" s="3" t="s">
         <v>3</v>
       </c>
@@ -1700,7 +1769,7 @@
         <v>20000</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" s="3" t="s">
         <v>3</v>
       </c>
@@ -1711,7 +1780,7 @@
         <v>23533.33</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" s="3" t="s">
         <v>3</v>
       </c>
@@ -1722,7 +1791,7 @@
         <v>20000</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" s="3" t="s">
         <v>3</v>
       </c>
@@ -1733,7 +1802,7 @@
         <v>22500</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" s="3" t="s">
         <v>3</v>
       </c>
@@ -1744,7 +1813,7 @@
         <v>22889.5</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" s="3" t="s">
         <v>3</v>
       </c>
@@ -1755,7 +1824,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" s="3" t="s">
         <v>3</v>
       </c>
@@ -1766,7 +1835,7 @@
         <v>12096</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" s="3" t="s">
         <v>3</v>
       </c>
@@ -1777,7 +1846,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" s="3" t="s">
         <v>3</v>
       </c>
@@ -1788,7 +1857,7 @@
         <v>12096</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" s="3" t="s">
         <v>3</v>
       </c>
@@ -1799,7 +1868,7 @@
         <v>29336.5</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" s="3" t="s">
         <v>3</v>
       </c>
@@ -1810,7 +1879,7 @@
         <v>25200</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" s="3" t="s">
         <v>3</v>
       </c>
@@ -1821,7 +1890,7 @@
         <v>29336.5</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" s="3" t="s">
         <v>6</v>
       </c>
@@ -1832,7 +1901,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" s="3" t="s">
         <v>6</v>
       </c>
@@ -1843,7 +1912,7 @@
         <v>410.32499999999999</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" s="3" t="s">
         <v>6</v>
       </c>
@@ -1854,7 +1923,7 @@
         <v>958.2</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" s="3" t="s">
         <v>6</v>
       </c>
@@ -1865,7 +1934,7 @@
         <v>1295.04</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" s="3" t="s">
         <v>6</v>
       </c>
@@ -1876,7 +1945,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" s="3" t="s">
         <v>6</v>
       </c>
@@ -1887,7 +1956,7 @@
         <v>1934.02</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" s="3" t="s">
         <v>6</v>
       </c>
@@ -1898,7 +1967,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" s="3" t="s">
         <v>6</v>
       </c>
@@ -1909,7 +1978,7 @@
         <v>3800</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" s="3" t="s">
         <v>6</v>
       </c>
@@ -1920,7 +1989,7 @@
         <v>3957.0947632342136</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" s="3" t="s">
         <v>6</v>
       </c>
@@ -1931,7 +2000,7 @@
         <v>4759.0511791608687</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" s="3" t="s">
         <v>6</v>
       </c>
@@ -1942,7 +2011,7 @@
         <v>6240.3966749700603</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" s="3" t="s">
         <v>6</v>
       </c>
@@ -1953,7 +2022,7 @@
         <v>2089.1907460551201</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" s="3" t="s">
         <v>6</v>
       </c>
@@ -1964,7 +2033,7 @@
         <v>2413.0790910766741</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" s="3" t="s">
         <v>6</v>
       </c>
@@ -1975,7 +2044,7 @@
         <v>3064.7380044333945</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" s="3" t="s">
         <v>6</v>
       </c>
@@ -1986,7 +2055,7 @@
         <v>3957.0947632342136</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" s="3" t="s">
         <v>6</v>
       </c>
@@ -1997,7 +2066,7 @@
         <v>4135.1224323299648</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" s="3" t="s">
         <v>6</v>
       </c>
@@ -2008,7 +2077,7 @@
         <v>5019.7147445035562</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" s="3" t="s">
         <v>6</v>
       </c>
@@ -2019,7 +2088,7 @@
         <v>6232.0776250123145</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" s="3" t="s">
         <v>6</v>
       </c>
@@ -2030,7 +2099,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109" s="3" t="s">
         <v>6</v>
       </c>
@@ -2041,7 +2110,7 @@
         <v>945</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110" s="3" t="s">
         <v>6</v>
       </c>
@@ -2052,7 +2121,7 @@
         <v>850.56999999999994</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" s="3" t="s">
         <v>6</v>
       </c>
@@ -2063,7 +2132,7 @@
         <v>1237.5</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112" s="3" t="s">
         <v>6</v>
       </c>
@@ -2074,7 +2143,7 @@
         <v>998.93</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" s="3" t="s">
         <v>6</v>
       </c>
@@ -2085,7 +2154,7 @@
         <v>1431.41</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" s="3" t="s">
         <v>6</v>
       </c>
@@ -2096,7 +2165,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" s="3" t="s">
         <v>6</v>
       </c>
@@ -2107,7 +2176,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" s="3" t="s">
         <v>6</v>
       </c>
@@ -2118,7 +2187,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" s="3" t="s">
         <v>6</v>
       </c>
@@ -2129,7 +2198,7 @@
         <v>1290</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" s="3" t="s">
         <v>6</v>
       </c>
@@ -2140,7 +2209,7 @@
         <v>2780</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" s="3" t="s">
         <v>6</v>
       </c>
@@ -2151,7 +2220,7 @@
         <v>2980</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" s="3" t="s">
         <v>6</v>
       </c>
@@ -2162,7 +2231,7 @@
         <v>4800</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" s="3" t="s">
         <v>6</v>
       </c>
@@ -2173,7 +2242,7 @@
         <v>6735</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" s="3" t="s">
         <v>6</v>
       </c>
@@ -2184,18 +2253,21 @@
         <v>8100</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A123" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B123" s="5" t="s">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A123" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B123" s="22" t="s">
         <v>129</v>
       </c>
-      <c r="C123" s="7">
+      <c r="C123" s="19">
         <v>1263</v>
       </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D123" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" s="3" t="s">
         <v>6</v>
       </c>
@@ -2206,7 +2278,7 @@
         <v>1256</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" s="3" t="s">
         <v>6</v>
       </c>
@@ -2217,7 +2289,7 @@
         <v>1646.2733333333333</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126" s="3" t="s">
         <v>6</v>
       </c>
@@ -2228,7 +2300,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127" s="3" t="s">
         <v>6</v>
       </c>
@@ -2239,7 +2311,7 @@
         <v>2206.3775000000001</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128" s="3" t="s">
         <v>6</v>
       </c>
@@ -2250,7 +2322,7 @@
         <v>3440</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A129" s="3" t="s">
         <v>6</v>
       </c>
@@ -2261,7 +2333,7 @@
         <v>4540</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A130" s="3" t="s">
         <v>6</v>
       </c>
@@ -2272,7 +2344,7 @@
         <v>9150</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A131" s="3" t="s">
         <v>6</v>
       </c>
@@ -2283,7 +2355,7 @@
         <v>11620</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A132" s="3" t="s">
         <v>6</v>
       </c>
@@ -2294,7 +2366,7 @@
         <v>12600</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A133" s="3" t="s">
         <v>6</v>
       </c>
@@ -2305,7 +2377,7 @@
         <v>1578</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A134" s="3" t="s">
         <v>6</v>
       </c>
@@ -2316,7 +2388,7 @@
         <v>7320</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A135" s="3" t="s">
         <v>6</v>
       </c>
@@ -2327,7 +2399,7 @@
         <v>8070</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A136" s="3" t="s">
         <v>6</v>
       </c>
@@ -2338,7 +2410,7 @@
         <v>8950</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A137" s="3" t="s">
         <v>6</v>
       </c>
@@ -2349,7 +2421,7 @@
         <v>9570</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A138" s="3" t="s">
         <v>6</v>
       </c>
@@ -2360,7 +2432,7 @@
         <v>11810</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A139" s="3" t="s">
         <v>6</v>
       </c>

</xml_diff>